<commit_message>
Agent 6 Data Update
New potentially useful graph (the project description is a little vague), and corresponding calculations in spreadsheet
</commit_message>
<xml_diff>
--- a/Agent 6 Data.xlsx
+++ b/Agent 6 Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacht\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacht\OneDrive\Desktop\CS520-Probability-in-Grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E34FD10-03B7-4B13-A3B7-F47C9AA8CF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231A6A15-FE1D-4D03-A558-847C4907181C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7908A210-88CB-4249-BDA8-5DC3DEC7C714}"/>
+    <workbookView xWindow="0" yWindow="1146" windowWidth="17280" windowHeight="8994" xr2:uid="{7908A210-88CB-4249-BDA8-5DC3DEC7C714}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Examinations</t>
   </si>
   <si>
     <t>Collisions (included in trajectory length, but shown here as well)</t>
-  </si>
-  <si>
-    <t>Trajectory Length (movements + collisions)</t>
   </si>
   <si>
     <t>Total Cost (trajectory length + collision)</t>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>Averages</t>
+  </si>
+  <si>
+    <t>Trajectory Length / Examinations</t>
+  </si>
+  <si>
+    <t>Trajectory Length (aka movements)</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433620E7-D7B7-4828-9E14-8CF114097915}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -419,11 +422,12 @@
     <col min="3" max="3" width="13.1015625" customWidth="1"/>
     <col min="4" max="4" width="15.3671875" customWidth="1"/>
     <col min="5" max="5" width="14.7890625" customWidth="1"/>
+    <col min="7" max="7" width="17.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -432,13 +436,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>228240</v>
       </c>
@@ -455,8 +462,12 @@
       <c r="E2">
         <v>60.973999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2">
+        <f>A2/C2</f>
+        <v>9.0427892234548342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>623931</v>
       </c>
@@ -473,8 +484,12 @@
       <c r="E3">
         <v>67.397000000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3">
+        <f t="shared" ref="G3:G51" si="1">A3/C3</f>
+        <v>11.990372050119149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>139567</v>
       </c>
@@ -491,8 +506,12 @@
       <c r="E4">
         <v>51.912999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>7.5637871233470628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>1373</v>
       </c>
@@ -509,8 +528,12 @@
       <c r="E5">
         <v>3.0640000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>2.9088983050847457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5499</v>
       </c>
@@ -527,8 +550,12 @@
       <c r="E6">
         <v>7.742</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2.9596340150699678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>37414</v>
       </c>
@@ -545,8 +572,12 @@
       <c r="E7">
         <v>73.44</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4.5743978481476955</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>214734</v>
       </c>
@@ -563,8 +594,12 @@
       <c r="E8">
         <v>55.816000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>8.9775492286466818</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>1118</v>
       </c>
@@ -581,8 +616,12 @@
       <c r="E9">
         <v>1.07</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2.830379746835443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>462247</v>
       </c>
@@ -599,8 +638,12 @@
       <c r="E10">
         <v>77.278000000000006</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>10.611487339592754</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>458467</v>
       </c>
@@ -617,8 +660,12 @@
       <c r="E11">
         <v>90.680999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>11.227579957878239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>16941</v>
       </c>
@@ -635,8 +682,12 @@
       <c r="E12">
         <v>32.276000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>3.0187099073414112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>21192</v>
       </c>
@@ -653,8 +704,12 @@
       <c r="E13">
         <v>86.358999999999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>3.1848512173128944</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>9579</v>
       </c>
@@ -671,8 +726,12 @@
       <c r="E14">
         <v>36.222000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>3.043851286939943</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>63269</v>
       </c>
@@ -689,8 +748,12 @@
       <c r="E15">
         <v>58.045000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>5.9564112219920915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>18591</v>
       </c>
@@ -707,8 +770,12 @@
       <c r="E16">
         <v>26.748999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>3.0342745226048637</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>278841</v>
       </c>
@@ -725,8 +792,12 @@
       <c r="E17">
         <v>64.090999999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>9.9146991893045087</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>273051</v>
       </c>
@@ -743,8 +814,12 @@
       <c r="E18">
         <v>56.506999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>8.7775170374180274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>9839</v>
       </c>
@@ -761,8 +836,12 @@
       <c r="E19">
         <v>12.752000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>2.9335122242098985</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>5803</v>
       </c>
@@ -779,8 +858,12 @@
       <c r="E20">
         <v>12.526999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>3.1675764192139737</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>539779</v>
       </c>
@@ -797,8 +880,12 @@
       <c r="E21">
         <v>77.561999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>12.132591593616542</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>12165</v>
       </c>
@@ -815,8 +902,12 @@
       <c r="E22">
         <v>19.318999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>3.0867800050748539</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>4546</v>
       </c>
@@ -833,8 +924,12 @@
       <c r="E23">
         <v>6.7990000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>3.0066137566137567</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>196253</v>
       </c>
@@ -851,8 +946,12 @@
       <c r="E24">
         <v>63.604999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>8.6953035002215326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>11962</v>
       </c>
@@ -869,8 +968,12 @@
       <c r="E25">
         <v>18.734000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>2.9660302504339202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>641929</v>
       </c>
@@ -887,8 +990,12 @@
       <c r="E26">
         <v>88.807000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>11.185185830530919</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>286457</v>
       </c>
@@ -905,8 +1012,12 @@
       <c r="E27">
         <v>79.034999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>9.6619333513221797</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>60231</v>
       </c>
@@ -923,8 +1034,12 @@
       <c r="E28">
         <v>76.718000000000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>5.6956028368794325</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>15070</v>
       </c>
@@ -941,8 +1056,12 @@
       <c r="E29">
         <v>26.821000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>3.000199084212622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>107191</v>
       </c>
@@ -959,8 +1078,12 @@
       <c r="E30">
         <v>70.724999999999994</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>7.7730964467005075</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>101190</v>
       </c>
@@ -977,8 +1100,12 @@
       <c r="E31">
         <v>81.063999999999993</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>6.896340216724596</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>578821</v>
       </c>
@@ -995,8 +1122,12 @@
       <c r="E32">
         <v>77.063999999999993</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>11.331212560197329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>18940</v>
       </c>
@@ -1013,8 +1144,12 @@
       <c r="E33">
         <v>27.888999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>3.0053951126626468</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>22497</v>
       </c>
@@ -1031,8 +1166,12 @@
       <c r="E34">
         <v>48.116</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>3.2379101899827289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>2422</v>
       </c>
@@ -1049,8 +1188,12 @@
       <c r="E35">
         <v>3.8820000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>2.94647201946472</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>63774</v>
       </c>
@@ -1067,8 +1210,12 @@
       <c r="E36">
         <v>64.506</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>6.0911174785100286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>12174</v>
       </c>
@@ -1085,8 +1232,12 @@
       <c r="E37">
         <v>25.369</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>3.0796863141917532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>119634</v>
       </c>
@@ -1103,8 +1254,12 @@
       <c r="E38">
         <v>70.75</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>7.2823228634039445</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>2633</v>
       </c>
@@ -1121,8 +1276,12 @@
       <c r="E39">
         <v>64.221999999999994</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>2.8902305159165751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>6155</v>
       </c>
@@ -1139,8 +1298,12 @@
       <c r="E40">
         <v>36.865000000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>3.1164556962025318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>19968</v>
       </c>
@@ -1157,8 +1320,12 @@
       <c r="E41">
         <v>39.808</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>3.0857672693555864</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>12318</v>
       </c>
@@ -1175,8 +1342,12 @@
       <c r="E42">
         <v>24.361000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>3.0302583025830256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>53201</v>
       </c>
@@ -1193,8 +1364,12 @@
       <c r="E43">
         <v>48.758000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>5.3522132796780681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>3813</v>
       </c>
@@ -1211,8 +1386,12 @@
       <c r="E44">
         <v>7.577</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>2.9535243996901626</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>144366</v>
       </c>
@@ -1229,8 +1408,12 @@
       <c r="E45">
         <v>65.518000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>7.8647853562867729</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>19242</v>
       </c>
@@ -1247,8 +1430,12 @@
       <c r="E46">
         <v>56.884</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>3.0586552217453504</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>19001</v>
       </c>
@@ -1265,8 +1452,12 @@
       <c r="E47">
         <v>26.061</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>3.0770850202429152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>251304</v>
       </c>
@@ -1283,8 +1474,12 @@
       <c r="E48">
         <v>68.462000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>9.0769341905656287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>21219</v>
       </c>
@@ -1301,8 +1496,12 @@
       <c r="E49">
         <v>42.625</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>3.1760215536596319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>263953</v>
       </c>
@@ -1319,8 +1518,12 @@
       <c r="E50">
         <v>64.367999999999995</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>9.2349380729130228</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>573891</v>
       </c>
@@ -1337,31 +1540,35 @@
       <c r="E51">
         <v>46.988999999999997</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>12.408454054054054</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <f>AVERAGE(A2:A51)</f>
         <v>141115.9</v>
       </c>
       <c r="B54">
-        <f t="shared" ref="B54:E54" si="1">AVERAGE(B2:B51)</f>
+        <f t="shared" ref="B54:E54" si="2">AVERAGE(B2:B51)</f>
         <v>2272.8200000000002</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15597.02</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156712.92000000001</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.883320000000005</v>
       </c>
     </row>

</xml_diff>